<commit_message>
Fill empty cells in filled rows
</commit_message>
<xml_diff>
--- a/test/xlsx/dataimages.xlsx
+++ b/test/xlsx/dataimages.xlsx
@@ -11,12 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Nullam aliquet mi et nunc tempus rutrum.</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -249,9 +246,7 @@
       <c r="C1">
         <v>260</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
+      <c r="D1"/>
     </row>
     <row r="2">
       <c r="A2">
@@ -263,9 +258,7 @@
       <c r="C2">
         <v>260</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2"/>
     </row>
     <row r="3">
       <c r="A3">
@@ -277,9 +270,7 @@
       <c r="C3">
         <v>260</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3"/>
     </row>
     <row r="4">
       <c r="A4">
@@ -291,9 +282,7 @@
       <c r="C4">
         <v>260</v>
       </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4"/>
     </row>
     <row r="5">
       <c r="A5">

</xml_diff>